<commit_message>
he añadido y gestionado los resultados del LSWI y he avanzado en el modelo para analizar los datos
</commit_message>
<xml_diff>
--- a/R/ResultadosR_LSWI.xlsx
+++ b/R/ResultadosR_LSWI.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VE-UGR-0208\Desktop\TFM\rTFM\R\LSWI_zones\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VE-UGR-0208\Desktop\TFM\rTFM\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17934538-7B74-467F-8BEC-520E4F4566B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E53AB4-629F-44A1-9599-CC846CF9BCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,33 @@
     <sheet name="MK" sheetId="4" r:id="rId3"/>
     <sheet name="lm() R2 y p-value" sheetId="3" r:id="rId4"/>
     <sheet name="Summary" sheetId="2" r:id="rId5"/>
+    <sheet name="Resultados 27-08" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Resultados 27-08'!$K$1:$R$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="998" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="404">
   <si>
     <t>Dado que el p-valor es menor que 0.05, rechazamos la hipótesis nula de que no hay tendencia monotónica en la serie de tiempo. Esto significa que hay evidencia estadísticamente significativa para concluir que existe una tendencia monotónica en la serie de tiempo.</t>
   </si>
@@ -1049,12 +1064,304 @@
   <si>
     <t>zone8: p-valor muy próximo a 0,05. ¿Es fiable?</t>
   </si>
+  <si>
+    <t>intercept_lm</t>
+  </si>
+  <si>
+    <t>slope_lm</t>
+  </si>
+  <si>
+    <t>p_value_slope</t>
+  </si>
+  <si>
+    <t>r_squared</t>
+  </si>
+  <si>
+    <t>adj_r_squared</t>
+  </si>
+  <si>
+    <t>tau_mk_test_2</t>
+  </si>
+  <si>
+    <t>p_value_mk_test_2</t>
+  </si>
+  <si>
+    <t>zone01b</t>
+  </si>
+  <si>
+    <t>zone02b</t>
+  </si>
+  <si>
+    <t>zone03b</t>
+  </si>
+  <si>
+    <t>zone04b</t>
+  </si>
+  <si>
+    <t>zone05b</t>
+  </si>
+  <si>
+    <t>zone06b</t>
+  </si>
+  <si>
+    <t>zone07b</t>
+  </si>
+  <si>
+    <t>zone08b</t>
+  </si>
+  <si>
+    <t>zone09b</t>
+  </si>
+  <si>
+    <t>zone10b</t>
+  </si>
+  <si>
+    <t>zone11b</t>
+  </si>
+  <si>
+    <t>zone12b</t>
+  </si>
+  <si>
+    <t>zone13b</t>
+  </si>
+  <si>
+    <t>zone14b</t>
+  </si>
+  <si>
+    <t>zone15b</t>
+  </si>
+  <si>
+    <t>zone01</t>
+  </si>
+  <si>
+    <t>zone02</t>
+  </si>
+  <si>
+    <t>zone03</t>
+  </si>
+  <si>
+    <t>zone04</t>
+  </si>
+  <si>
+    <t>zone05</t>
+  </si>
+  <si>
+    <t>zone06</t>
+  </si>
+  <si>
+    <t>zone07</t>
+  </si>
+  <si>
+    <t>zone08</t>
+  </si>
+  <si>
+    <t>zone09</t>
+  </si>
+  <si>
+    <t>Intercepto</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ajustado</t>
+    </r>
+  </si>
+  <si>
+    <t>Tau</t>
+  </si>
+  <si>
+    <t>P-valor Mann-Kendall</t>
+  </si>
+  <si>
+    <t>P-valor lm</t>
+  </si>
+  <si>
+    <t>ZONAS</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF3F3F3F"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ajustado</t>
+    </r>
+  </si>
+  <si>
+    <t>Albufera Honda (humedal)</t>
+  </si>
+  <si>
+    <t>Albufera Honda (buffer)</t>
+  </si>
+  <si>
+    <t>Albufera Nueva (humedal)</t>
+  </si>
+  <si>
+    <t>Albufera Nueva (buffer)</t>
+  </si>
+  <si>
+    <t>Barranco del Agua (humedal)</t>
+  </si>
+  <si>
+    <t>Barranco del Agua (buffer)</t>
+  </si>
+  <si>
+    <t>Cañada de las Norias (humedal)</t>
+  </si>
+  <si>
+    <t>Cañada de las Norias (buffer)</t>
+  </si>
+  <si>
+    <t>Charcones de Punta-Entinas (humedal)</t>
+  </si>
+  <si>
+    <t>Charcones de Punta-Entinas (buffer)</t>
+  </si>
+  <si>
+    <t>Cola del embalse del Negratín (humedal)</t>
+  </si>
+  <si>
+    <t>Cola del embalse del Negratín (buffer)</t>
+  </si>
+  <si>
+    <t>Humedales de Baza (humedal)</t>
+  </si>
+  <si>
+    <t>Humedales de Baza (buffer)</t>
+  </si>
+  <si>
+    <t>Laguna de la Gravera (humedal)</t>
+  </si>
+  <si>
+    <t>Laguna de la Gravera (buffer)</t>
+  </si>
+  <si>
+    <t>Rambla Morales (humedal)</t>
+  </si>
+  <si>
+    <t>Rambla Morales (buffer)</t>
+  </si>
+  <si>
+    <t>Ribera de la Algaida (humedal)</t>
+  </si>
+  <si>
+    <t>Ribera de la Algaida (buffer)</t>
+  </si>
+  <si>
+    <t>Río Antas (humedal)</t>
+  </si>
+  <si>
+    <t>Río Antas (buffer)</t>
+  </si>
+  <si>
+    <t>Saladar del Margen (humedal)</t>
+  </si>
+  <si>
+    <t>Saladar del Margen (buffer)</t>
+  </si>
+  <si>
+    <t>Salar de los Canos (humedal)</t>
+  </si>
+  <si>
+    <t>Salar de los Canos (buffer)</t>
+  </si>
+  <si>
+    <t>Salinas de Cabo de Gata (humedal)</t>
+  </si>
+  <si>
+    <t>Salinas de Cabo de Gata (buffer)</t>
+  </si>
+  <si>
+    <t>Salinas de Cerrillos (humedal)</t>
+  </si>
+  <si>
+    <t>Salinas de Cerrillos (buffer)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1079,8 +1386,40 @@
       <name val="Lucida Console"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1117,8 +1456,31 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59996337778862885"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1284,11 +1646,185 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1360,11 +1896,110 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="21" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="19" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="23" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="24" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="26" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="27" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="15" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -54210,7 +54845,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E45" sqref="E45"/>
     </sheetView>
   </sheetViews>
@@ -55153,7 +55788,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:G37">
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -55182,7 +55817,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:P24">
-    <cfRule type="cellIs" dxfId="0" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -55213,4 +55848,1844 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A47893D5-6C91-4DB8-9C3D-71AEB2F4F097}">
+  <dimension ref="A1:T32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:R31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" style="7" customWidth="1"/>
+    <col min="2" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="16.2" x14ac:dyDescent="0.3">
+      <c r="B1" s="37" t="s">
+        <v>364</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>365</v>
+      </c>
+      <c r="D1" s="37" t="s">
+        <v>370</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>367</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>368</v>
+      </c>
+      <c r="H1" s="37" t="s">
+        <v>369</v>
+      </c>
+      <c r="K1" s="70" t="s">
+        <v>371</v>
+      </c>
+      <c r="L1" s="71" t="s">
+        <v>364</v>
+      </c>
+      <c r="M1" s="71" t="s">
+        <v>365</v>
+      </c>
+      <c r="N1" s="71" t="s">
+        <v>370</v>
+      </c>
+      <c r="O1" s="71" t="s">
+        <v>372</v>
+      </c>
+      <c r="P1" s="71" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q1" s="71" t="s">
+        <v>368</v>
+      </c>
+      <c r="R1" s="71" t="s">
+        <v>369</v>
+      </c>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A2" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="B2" s="40">
+        <v>-0.86999614300000006</v>
+      </c>
+      <c r="C2" s="39">
+        <v>4.7618200000000002E-4</v>
+      </c>
+      <c r="D2" s="40">
+        <v>0.28383883599999998</v>
+      </c>
+      <c r="E2" s="41">
+        <v>5.4467572999999998E-2</v>
+      </c>
+      <c r="F2" s="41">
+        <v>9.4422199999999994E-3</v>
+      </c>
+      <c r="G2" s="40">
+        <v>0.185770765</v>
+      </c>
+      <c r="H2" s="40">
+        <v>0.22441148799999999</v>
+      </c>
+      <c r="I2" s="72" t="s">
+        <v>340</v>
+      </c>
+      <c r="K2" s="76" t="s">
+        <v>374</v>
+      </c>
+      <c r="L2" s="59">
+        <v>-1.9639655949999999</v>
+      </c>
+      <c r="M2" s="58">
+        <v>1.022231E-3</v>
+      </c>
+      <c r="N2" s="59">
+        <v>2.8864060000000002E-3</v>
+      </c>
+      <c r="O2" s="60">
+        <v>0.35115523999999998</v>
+      </c>
+      <c r="P2" s="60">
+        <v>0.32025787100000003</v>
+      </c>
+      <c r="Q2" s="59">
+        <v>0.38339921799999999</v>
+      </c>
+      <c r="R2" s="59">
+        <v>1.123178E-2</v>
+      </c>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A3" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="B3" s="40">
+        <v>-0.52144208400000003</v>
+      </c>
+      <c r="C3" s="39">
+        <v>2.9892800000000001E-4</v>
+      </c>
+      <c r="D3" s="40">
+        <v>0.45758387499999997</v>
+      </c>
+      <c r="E3" s="41">
+        <v>2.6548741000000001E-2</v>
+      </c>
+      <c r="F3" s="41">
+        <v>-1.9806081E-2</v>
+      </c>
+      <c r="G3" s="40">
+        <v>9.0909093999999996E-2</v>
+      </c>
+      <c r="H3" s="40">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="I3" s="72" t="s">
+        <v>341</v>
+      </c>
+      <c r="K3" s="77" t="s">
+        <v>375</v>
+      </c>
+      <c r="L3" s="40">
+        <v>-0.86999614300000006</v>
+      </c>
+      <c r="M3" s="39">
+        <v>4.7618200000000002E-4</v>
+      </c>
+      <c r="N3" s="40">
+        <v>0.28383883599999998</v>
+      </c>
+      <c r="O3" s="41">
+        <v>5.4467572999999998E-2</v>
+      </c>
+      <c r="P3" s="41">
+        <v>9.4422199999999994E-3</v>
+      </c>
+      <c r="Q3" s="40">
+        <v>0.185770765</v>
+      </c>
+      <c r="R3" s="40">
+        <v>0.22441148799999999</v>
+      </c>
+      <c r="S3" s="75"/>
+      <c r="T3" s="75"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A4" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="B4" s="40">
+        <v>-3.6383769999999999E-3</v>
+      </c>
+      <c r="C4" s="14">
+        <v>-3.1498700000000001E-6</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0.99055988100000003</v>
+      </c>
+      <c r="E4" s="41">
+        <v>6.8267000000000002E-6</v>
+      </c>
+      <c r="F4" s="41">
+        <v>-4.7611896000000001E-2</v>
+      </c>
+      <c r="G4" s="40">
+        <v>-3.9525690000000004E-3</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" s="72" t="s">
+        <v>342</v>
+      </c>
+      <c r="K4" s="76" t="s">
+        <v>376</v>
+      </c>
+      <c r="L4" s="40">
+        <v>0.13238884100000001</v>
+      </c>
+      <c r="M4" s="14">
+        <v>-4.4985699999999999E-5</v>
+      </c>
+      <c r="N4" s="40">
+        <v>0.80242258899999996</v>
+      </c>
+      <c r="O4" s="41">
+        <v>3.0483979999999999E-3</v>
+      </c>
+      <c r="P4" s="41">
+        <v>-4.4425487999999999E-2</v>
+      </c>
+      <c r="Q4" s="40">
+        <v>5.9288542999999999E-2</v>
+      </c>
+      <c r="R4" s="40">
+        <v>0.71157145499999996</v>
+      </c>
+      <c r="S4" s="75"/>
+      <c r="T4" s="75"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A5" s="72" t="s">
+        <v>343</v>
+      </c>
+      <c r="B5" s="40">
+        <v>-1.2290135040000001</v>
+      </c>
+      <c r="C5" s="39">
+        <v>6.4344800000000002E-4</v>
+      </c>
+      <c r="D5" s="40">
+        <v>0.20722028200000001</v>
+      </c>
+      <c r="E5" s="41">
+        <v>7.4630236000000003E-2</v>
+      </c>
+      <c r="F5" s="41">
+        <v>3.0565009000000001E-2</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0.28853756200000003</v>
+      </c>
+      <c r="H5" s="40">
+        <v>5.7229637999999999E-2</v>
+      </c>
+      <c r="I5" s="72" t="s">
+        <v>343</v>
+      </c>
+      <c r="K5" s="77" t="s">
+        <v>377</v>
+      </c>
+      <c r="L5" s="40">
+        <v>-0.52144208400000003</v>
+      </c>
+      <c r="M5" s="39">
+        <v>2.9892800000000001E-4</v>
+      </c>
+      <c r="N5" s="40">
+        <v>0.45758387499999997</v>
+      </c>
+      <c r="O5" s="41">
+        <v>2.6548741000000001E-2</v>
+      </c>
+      <c r="P5" s="41">
+        <v>-1.9806081E-2</v>
+      </c>
+      <c r="Q5" s="40">
+        <v>9.0909093999999996E-2</v>
+      </c>
+      <c r="R5" s="40">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="S5" s="75"/>
+      <c r="T5" s="75"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A6" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="B6" s="44">
+        <v>-0.82173034199999995</v>
+      </c>
+      <c r="C6" s="47">
+        <v>4.2273499999999998E-4</v>
+      </c>
+      <c r="D6" s="48">
+        <v>3.0678654E-2</v>
+      </c>
+      <c r="E6" s="49">
+        <v>0.20361601200000001</v>
+      </c>
+      <c r="F6" s="50">
+        <v>0.165692965</v>
+      </c>
+      <c r="G6" s="40">
+        <v>0.264822155</v>
+      </c>
+      <c r="H6" s="40">
+        <v>8.1317901999999997E-2</v>
+      </c>
+      <c r="I6" s="72" t="s">
+        <v>344</v>
+      </c>
+      <c r="K6" s="76" t="s">
+        <v>378</v>
+      </c>
+      <c r="L6" s="48">
+        <v>0.27755689099999997</v>
+      </c>
+      <c r="M6" s="47">
+        <v>-1.37575E-4</v>
+      </c>
+      <c r="N6" s="48">
+        <v>0.69677338300000002</v>
+      </c>
+      <c r="O6" s="49">
+        <v>7.3776709999999997E-3</v>
+      </c>
+      <c r="P6" s="50">
+        <v>-3.9890058999999999E-2</v>
+      </c>
+      <c r="Q6" s="40">
+        <v>-9.0909093999999996E-2</v>
+      </c>
+      <c r="R6" s="40">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="S6" s="75"/>
+      <c r="T6" s="75"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A7" s="72" t="s">
+        <v>345</v>
+      </c>
+      <c r="B7" s="40">
+        <v>0.1322248</v>
+      </c>
+      <c r="C7" s="14">
+        <v>-6.2291099999999997E-5</v>
+      </c>
+      <c r="D7" s="40">
+        <v>0.88892369400000004</v>
+      </c>
+      <c r="E7" s="41">
+        <v>9.5080800000000004E-4</v>
+      </c>
+      <c r="F7" s="41">
+        <v>-4.6622963000000003E-2</v>
+      </c>
+      <c r="G7" s="40">
+        <v>6.7193680000000006E-2</v>
+      </c>
+      <c r="H7" s="40">
+        <v>0.67261099800000002</v>
+      </c>
+      <c r="I7" s="72" t="s">
+        <v>345</v>
+      </c>
+      <c r="K7" s="77" t="s">
+        <v>379</v>
+      </c>
+      <c r="L7" s="40">
+        <v>-3.6383769999999999E-3</v>
+      </c>
+      <c r="M7" s="14">
+        <v>-3.1498700000000001E-6</v>
+      </c>
+      <c r="N7" s="40">
+        <v>0.99055988100000003</v>
+      </c>
+      <c r="O7" s="41">
+        <v>6.8267000000000002E-6</v>
+      </c>
+      <c r="P7" s="41">
+        <v>-4.7611896000000001E-2</v>
+      </c>
+      <c r="Q7" s="40">
+        <v>-3.9525690000000004E-3</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7" s="75"/>
+      <c r="T7" s="75"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A8" s="72" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="40">
+        <v>-9.2534265000000004E-2</v>
+      </c>
+      <c r="C8" s="14">
+        <v>5.9288199999999999E-5</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.89280802199999998</v>
+      </c>
+      <c r="E8" s="41">
+        <v>8.8510300000000004E-4</v>
+      </c>
+      <c r="F8" s="41">
+        <v>-4.6691796000000001E-2</v>
+      </c>
+      <c r="G8" s="40">
+        <v>0.122529648</v>
+      </c>
+      <c r="H8" s="40">
+        <v>0.42817783399999998</v>
+      </c>
+      <c r="I8" s="72" t="s">
+        <v>346</v>
+      </c>
+      <c r="K8" s="76" t="s">
+        <v>380</v>
+      </c>
+      <c r="L8" s="40">
+        <v>0.57829115399999997</v>
+      </c>
+      <c r="M8" s="39">
+        <v>-2.6350899999999999E-4</v>
+      </c>
+      <c r="N8" s="40">
+        <v>0.27007952499999999</v>
+      </c>
+      <c r="O8" s="41">
+        <v>5.7584529000000002E-2</v>
+      </c>
+      <c r="P8" s="41">
+        <v>1.2707601000000001E-2</v>
+      </c>
+      <c r="Q8" s="40">
+        <v>-0.10671937500000001</v>
+      </c>
+      <c r="R8" s="40">
+        <v>0.492289484</v>
+      </c>
+      <c r="S8" s="75"/>
+      <c r="T8" s="75"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A9" s="72" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" s="44">
+        <v>-1.897600137</v>
+      </c>
+      <c r="C9" s="47">
+        <v>9.5440599999999998E-4</v>
+      </c>
+      <c r="D9" s="51">
+        <v>1.13078E-5</v>
+      </c>
+      <c r="E9" s="49">
+        <v>0.60869891099999995</v>
+      </c>
+      <c r="F9" s="50">
+        <v>0.59006552599999995</v>
+      </c>
+      <c r="G9" s="42">
+        <v>0.58893281200000003</v>
+      </c>
+      <c r="H9" s="43">
+        <v>9.2744799999999993E-5</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>347</v>
+      </c>
+      <c r="K9" s="77" t="s">
+        <v>381</v>
+      </c>
+      <c r="L9" s="48">
+        <v>-1.2290135040000001</v>
+      </c>
+      <c r="M9" s="47">
+        <v>6.4344800000000002E-4</v>
+      </c>
+      <c r="N9" s="48">
+        <v>0.20722028200000001</v>
+      </c>
+      <c r="O9" s="49">
+        <v>7.4630236000000003E-2</v>
+      </c>
+      <c r="P9" s="50">
+        <v>3.0565009000000001E-2</v>
+      </c>
+      <c r="Q9" s="42">
+        <v>0.28853756200000003</v>
+      </c>
+      <c r="R9" s="68">
+        <v>5.7229637999999999E-2</v>
+      </c>
+      <c r="S9" s="75"/>
+      <c r="T9" s="75"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A10" s="72" t="s">
+        <v>348</v>
+      </c>
+      <c r="B10" s="44">
+        <v>-1.5102784279999999</v>
+      </c>
+      <c r="C10" s="47">
+        <v>7.5302300000000002E-4</v>
+      </c>
+      <c r="D10" s="48">
+        <v>1.2362385E-2</v>
+      </c>
+      <c r="E10" s="49">
+        <v>0.26287368900000002</v>
+      </c>
+      <c r="F10" s="50">
+        <v>0.22777243599999999</v>
+      </c>
+      <c r="G10" s="44">
+        <v>0.35177868600000001</v>
+      </c>
+      <c r="H10" s="45">
+        <v>2.0119070999999999E-2</v>
+      </c>
+      <c r="I10" s="72" t="s">
+        <v>348</v>
+      </c>
+      <c r="K10" s="76" t="s">
+        <v>382</v>
+      </c>
+      <c r="L10" s="48">
+        <v>-3.7472046309999998</v>
+      </c>
+      <c r="M10" s="47">
+        <v>1.894778E-3</v>
+      </c>
+      <c r="N10" s="48">
+        <v>2.2268986000000001E-2</v>
+      </c>
+      <c r="O10" s="49">
+        <v>0.224815028</v>
+      </c>
+      <c r="P10" s="50">
+        <v>0.18790145799999999</v>
+      </c>
+      <c r="Q10" s="44">
+        <v>0.23320159300000001</v>
+      </c>
+      <c r="R10" s="45">
+        <v>0.125570178</v>
+      </c>
+      <c r="S10" s="75"/>
+      <c r="T10" s="75"/>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A11" s="72" t="s">
+        <v>349</v>
+      </c>
+      <c r="B11" s="40">
+        <v>7.9191103999999998E-2</v>
+      </c>
+      <c r="C11" s="14">
+        <v>-2.6781600000000001E-5</v>
+      </c>
+      <c r="D11" s="40">
+        <v>0.78432167500000005</v>
+      </c>
+      <c r="E11" s="41">
+        <v>3.6462270000000001E-3</v>
+      </c>
+      <c r="F11" s="41">
+        <v>-4.3799191000000001E-2</v>
+      </c>
+      <c r="G11" s="40">
+        <v>3.9525690000000004E-3</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" s="72" t="s">
+        <v>349</v>
+      </c>
+      <c r="K11" s="77" t="s">
+        <v>383</v>
+      </c>
+      <c r="L11" s="59">
+        <v>-0.82173034199999995</v>
+      </c>
+      <c r="M11" s="58">
+        <v>4.2273499999999998E-4</v>
+      </c>
+      <c r="N11" s="59">
+        <v>3.0678654E-2</v>
+      </c>
+      <c r="O11" s="60">
+        <v>0.20361601200000001</v>
+      </c>
+      <c r="P11" s="60">
+        <v>0.165692965</v>
+      </c>
+      <c r="Q11" s="40">
+        <v>0.264822155</v>
+      </c>
+      <c r="R11" s="40">
+        <v>8.1317901999999997E-2</v>
+      </c>
+      <c r="S11" s="75"/>
+      <c r="T11" s="75"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A12" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="B12" s="44">
+        <v>-2.4536090119999998</v>
+      </c>
+      <c r="C12" s="47">
+        <v>1.2248109999999999E-3</v>
+      </c>
+      <c r="D12" s="48">
+        <v>2.5473100000000001E-4</v>
+      </c>
+      <c r="E12" s="49">
+        <v>0.47872900000000002</v>
+      </c>
+      <c r="F12" s="50">
+        <v>0.45390657099999998</v>
+      </c>
+      <c r="G12" s="44">
+        <v>0.51778662200000003</v>
+      </c>
+      <c r="H12" s="45">
+        <v>5.9616599999999997E-4</v>
+      </c>
+      <c r="I12" s="72" t="s">
+        <v>350</v>
+      </c>
+      <c r="K12" s="76" t="s">
+        <v>384</v>
+      </c>
+      <c r="L12" s="48">
+        <v>3.697133279</v>
+      </c>
+      <c r="M12" s="47">
+        <v>-1.8153869999999999E-3</v>
+      </c>
+      <c r="N12" s="51">
+        <v>3.1511499999999998E-9</v>
+      </c>
+      <c r="O12" s="49">
+        <v>0.81829441999999997</v>
+      </c>
+      <c r="P12" s="50">
+        <v>0.80964177299999995</v>
+      </c>
+      <c r="Q12" s="44">
+        <v>-0.73122531199999996</v>
+      </c>
+      <c r="R12" s="46">
+        <v>1.17668E-6</v>
+      </c>
+      <c r="S12" s="75"/>
+      <c r="T12" s="75"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="72" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" s="40">
+        <v>-9.3546652999999994E-2</v>
+      </c>
+      <c r="C13" s="14">
+        <v>4.3538100000000002E-5</v>
+      </c>
+      <c r="D13" s="40">
+        <v>0.88769484399999998</v>
+      </c>
+      <c r="E13" s="41">
+        <v>9.7209300000000005E-4</v>
+      </c>
+      <c r="F13" s="41">
+        <v>-4.6600664999999999E-2</v>
+      </c>
+      <c r="G13" s="40">
+        <v>3.5573124999999997E-2</v>
+      </c>
+      <c r="H13" s="40">
+        <v>0.83266591999999995</v>
+      </c>
+      <c r="I13" s="72" t="s">
+        <v>351</v>
+      </c>
+      <c r="K13" s="77" t="s">
+        <v>385</v>
+      </c>
+      <c r="L13" s="40">
+        <v>0.1322248</v>
+      </c>
+      <c r="M13" s="14">
+        <v>-6.2291099999999997E-5</v>
+      </c>
+      <c r="N13" s="40">
+        <v>0.88892369400000004</v>
+      </c>
+      <c r="O13" s="41">
+        <v>9.5080800000000004E-4</v>
+      </c>
+      <c r="P13" s="41">
+        <v>-4.6622963000000003E-2</v>
+      </c>
+      <c r="Q13" s="40">
+        <v>6.7193680000000006E-2</v>
+      </c>
+      <c r="R13" s="40">
+        <v>0.67261099800000002</v>
+      </c>
+      <c r="S13" s="75"/>
+      <c r="T13" s="75"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A14" s="72" t="s">
+        <v>352</v>
+      </c>
+      <c r="B14" s="44">
+        <v>-2.842487363</v>
+      </c>
+      <c r="C14" s="47">
+        <v>1.41201E-3</v>
+      </c>
+      <c r="D14" s="51">
+        <v>1.05596E-5</v>
+      </c>
+      <c r="E14" s="49">
+        <v>0.61117614300000001</v>
+      </c>
+      <c r="F14" s="50">
+        <v>0.59266072199999997</v>
+      </c>
+      <c r="G14" s="44">
+        <v>0.62055337399999999</v>
+      </c>
+      <c r="H14" s="46">
+        <v>3.7908599999999998E-5</v>
+      </c>
+      <c r="I14" s="72" t="s">
+        <v>352</v>
+      </c>
+      <c r="K14" s="76" t="s">
+        <v>386</v>
+      </c>
+      <c r="L14" s="48">
+        <v>0.10871773899999999</v>
+      </c>
+      <c r="M14" s="51">
+        <v>-3.5629500000000002E-5</v>
+      </c>
+      <c r="N14" s="48">
+        <v>0.94820806000000002</v>
+      </c>
+      <c r="O14" s="49">
+        <v>2.05744E-4</v>
+      </c>
+      <c r="P14" s="50">
+        <v>-4.7403505999999998E-2</v>
+      </c>
+      <c r="Q14" s="44">
+        <v>-1.1857708E-2</v>
+      </c>
+      <c r="R14" s="45">
+        <v>0.95787459600000002</v>
+      </c>
+      <c r="S14" s="75"/>
+      <c r="T14" s="75"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A15" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="B15" s="53">
+        <v>-1.2682307159999999</v>
+      </c>
+      <c r="C15" s="54">
+        <v>6.3139100000000003E-4</v>
+      </c>
+      <c r="D15" s="55">
+        <v>2.4793835E-2</v>
+      </c>
+      <c r="E15" s="56">
+        <v>0.217743033</v>
+      </c>
+      <c r="F15" s="57">
+        <v>0.18049270100000001</v>
+      </c>
+      <c r="G15" s="44">
+        <v>0.32015812399999999</v>
+      </c>
+      <c r="H15" s="45">
+        <v>3.4614801000000001E-2</v>
+      </c>
+      <c r="I15" s="72" t="s">
+        <v>353</v>
+      </c>
+      <c r="K15" s="77" t="s">
+        <v>387</v>
+      </c>
+      <c r="L15" s="55">
+        <v>-9.2534265000000004E-2</v>
+      </c>
+      <c r="M15" s="67">
+        <v>5.9288199999999999E-5</v>
+      </c>
+      <c r="N15" s="55">
+        <v>0.89280802199999998</v>
+      </c>
+      <c r="O15" s="56">
+        <v>8.8510300000000004E-4</v>
+      </c>
+      <c r="P15" s="57">
+        <v>-4.6691796000000001E-2</v>
+      </c>
+      <c r="Q15" s="44">
+        <v>0.122529648</v>
+      </c>
+      <c r="R15" s="45">
+        <v>0.42817783399999998</v>
+      </c>
+      <c r="S15" s="75"/>
+      <c r="T15" s="75"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A16" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="B16" s="44">
+        <v>-1.868733872</v>
+      </c>
+      <c r="C16" s="47">
+        <v>9.5417799999999997E-4</v>
+      </c>
+      <c r="D16" s="48">
+        <v>8.0778229999999996E-3</v>
+      </c>
+      <c r="E16" s="49">
+        <v>0.28958943100000001</v>
+      </c>
+      <c r="F16" s="50">
+        <v>0.25576035600000002</v>
+      </c>
+      <c r="G16" s="44">
+        <v>0.37549409299999997</v>
+      </c>
+      <c r="H16" s="45">
+        <v>1.3043404E-2</v>
+      </c>
+      <c r="I16" s="72" t="s">
+        <v>354</v>
+      </c>
+      <c r="K16" s="76" t="s">
+        <v>388</v>
+      </c>
+      <c r="L16" s="48">
+        <v>-0.68686740700000004</v>
+      </c>
+      <c r="M16" s="47">
+        <v>3.58594E-4</v>
+      </c>
+      <c r="N16" s="48">
+        <v>4.9703561E-2</v>
+      </c>
+      <c r="O16" s="49">
+        <v>0.17117596900000001</v>
+      </c>
+      <c r="P16" s="50">
+        <v>0.13170815799999999</v>
+      </c>
+      <c r="Q16" s="44">
+        <v>0.24110673399999999</v>
+      </c>
+      <c r="R16" s="45">
+        <v>0.113050938</v>
+      </c>
+      <c r="S16" s="75"/>
+      <c r="T16" s="75"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A17" s="52" t="s">
+        <v>355</v>
+      </c>
+      <c r="B17" s="61">
+        <v>-1.9639655949999999</v>
+      </c>
+      <c r="C17" s="62">
+        <v>1.022231E-3</v>
+      </c>
+      <c r="D17" s="63">
+        <v>2.8864060000000002E-3</v>
+      </c>
+      <c r="E17" s="64">
+        <v>0.35115523999999998</v>
+      </c>
+      <c r="F17" s="65">
+        <v>0.32025787100000003</v>
+      </c>
+      <c r="G17" s="44">
+        <v>0.38339921799999999</v>
+      </c>
+      <c r="H17" s="45">
+        <v>1.123178E-2</v>
+      </c>
+      <c r="I17" s="74" t="s">
+        <v>355</v>
+      </c>
+      <c r="K17" s="77" t="s">
+        <v>389</v>
+      </c>
+      <c r="L17" s="63">
+        <v>-1.897600137</v>
+      </c>
+      <c r="M17" s="62">
+        <v>9.5440599999999998E-4</v>
+      </c>
+      <c r="N17" s="66">
+        <v>1.13078E-5</v>
+      </c>
+      <c r="O17" s="64">
+        <v>0.60869891099999995</v>
+      </c>
+      <c r="P17" s="65">
+        <v>0.59006552599999995</v>
+      </c>
+      <c r="Q17" s="44">
+        <v>0.58893281200000003</v>
+      </c>
+      <c r="R17" s="46">
+        <v>9.2744799999999993E-5</v>
+      </c>
+      <c r="S17" s="75"/>
+      <c r="T17" s="75"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A18" s="73" t="s">
+        <v>356</v>
+      </c>
+      <c r="B18" s="40">
+        <v>0.13238884100000001</v>
+      </c>
+      <c r="C18" s="14">
+        <v>-4.4985699999999999E-5</v>
+      </c>
+      <c r="D18" s="40">
+        <v>0.80242258899999996</v>
+      </c>
+      <c r="E18" s="41">
+        <v>3.0483979999999999E-3</v>
+      </c>
+      <c r="F18" s="41">
+        <v>-4.4425487999999999E-2</v>
+      </c>
+      <c r="G18" s="40">
+        <v>5.9288542999999999E-2</v>
+      </c>
+      <c r="H18" s="40">
+        <v>0.71157145499999996</v>
+      </c>
+      <c r="I18" s="74" t="s">
+        <v>356</v>
+      </c>
+      <c r="K18" s="76" t="s">
+        <v>390</v>
+      </c>
+      <c r="L18" s="40">
+        <v>1.1167735459999999</v>
+      </c>
+      <c r="M18" s="39">
+        <v>-5.1635799999999996E-4</v>
+      </c>
+      <c r="N18" s="40">
+        <v>0.32140079799999999</v>
+      </c>
+      <c r="O18" s="41">
+        <v>4.6812742999999997E-2</v>
+      </c>
+      <c r="P18" s="41">
+        <v>1.4228730000000001E-3</v>
+      </c>
+      <c r="Q18" s="40">
+        <v>-0.15415020300000001</v>
+      </c>
+      <c r="R18" s="40">
+        <v>0.31557267900000002</v>
+      </c>
+      <c r="S18" s="75"/>
+      <c r="T18" s="75"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A19" s="73" t="s">
+        <v>357</v>
+      </c>
+      <c r="B19" s="40">
+        <v>0.27755689099999997</v>
+      </c>
+      <c r="C19" s="39">
+        <v>-1.37575E-4</v>
+      </c>
+      <c r="D19" s="40">
+        <v>0.69677338300000002</v>
+      </c>
+      <c r="E19" s="41">
+        <v>7.3776709999999997E-3</v>
+      </c>
+      <c r="F19" s="41">
+        <v>-3.9890058999999999E-2</v>
+      </c>
+      <c r="G19" s="40">
+        <v>-9.0909093999999996E-2</v>
+      </c>
+      <c r="H19" s="40">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="I19" s="74" t="s">
+        <v>357</v>
+      </c>
+      <c r="K19" s="77" t="s">
+        <v>391</v>
+      </c>
+      <c r="L19" s="59">
+        <v>-1.5102784279999999</v>
+      </c>
+      <c r="M19" s="58">
+        <v>7.5302300000000002E-4</v>
+      </c>
+      <c r="N19" s="59">
+        <v>1.2362385E-2</v>
+      </c>
+      <c r="O19" s="60">
+        <v>0.26287368900000002</v>
+      </c>
+      <c r="P19" s="60">
+        <v>0.22777243599999999</v>
+      </c>
+      <c r="Q19" s="59">
+        <v>0.35177868600000001</v>
+      </c>
+      <c r="R19" s="59">
+        <v>2.0119070999999999E-2</v>
+      </c>
+      <c r="S19" s="75"/>
+      <c r="T19" s="75"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A20" s="73" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" s="40">
+        <v>0.57829115399999997</v>
+      </c>
+      <c r="C20" s="39">
+        <v>-2.6350899999999999E-4</v>
+      </c>
+      <c r="D20" s="40">
+        <v>0.27007952499999999</v>
+      </c>
+      <c r="E20" s="41">
+        <v>5.7584529000000002E-2</v>
+      </c>
+      <c r="F20" s="41">
+        <v>1.2707601000000001E-2</v>
+      </c>
+      <c r="G20" s="40">
+        <v>-0.10671937500000001</v>
+      </c>
+      <c r="H20" s="40">
+        <v>0.492289484</v>
+      </c>
+      <c r="I20" s="74" t="s">
+        <v>358</v>
+      </c>
+      <c r="K20" s="76" t="s">
+        <v>392</v>
+      </c>
+      <c r="L20" s="40">
+        <v>-0.82318983999999995</v>
+      </c>
+      <c r="M20" s="39">
+        <v>4.3709899999999998E-4</v>
+      </c>
+      <c r="N20" s="40">
+        <v>0.40334990300000001</v>
+      </c>
+      <c r="O20" s="41">
+        <v>3.3478521999999997E-2</v>
+      </c>
+      <c r="P20" s="41">
+        <v>-1.2546310999999999E-2</v>
+      </c>
+      <c r="Q20" s="40">
+        <v>0.114624515</v>
+      </c>
+      <c r="R20" s="40">
+        <v>0.45960783999999999</v>
+      </c>
+      <c r="S20" s="75"/>
+      <c r="T20" s="75"/>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A21" s="52" t="s">
+        <v>359</v>
+      </c>
+      <c r="B21" s="53">
+        <v>-3.7472046309999998</v>
+      </c>
+      <c r="C21" s="54">
+        <v>1.894778E-3</v>
+      </c>
+      <c r="D21" s="55">
+        <v>2.2268986000000001E-2</v>
+      </c>
+      <c r="E21" s="56">
+        <v>0.224815028</v>
+      </c>
+      <c r="F21" s="57">
+        <v>0.18790145799999999</v>
+      </c>
+      <c r="G21" s="40">
+        <v>0.23320159300000001</v>
+      </c>
+      <c r="H21" s="40">
+        <v>0.125570178</v>
+      </c>
+      <c r="I21" s="74" t="s">
+        <v>359</v>
+      </c>
+      <c r="K21" s="77" t="s">
+        <v>393</v>
+      </c>
+      <c r="L21" s="55">
+        <v>7.9191103999999998E-2</v>
+      </c>
+      <c r="M21" s="67">
+        <v>-2.6781600000000001E-5</v>
+      </c>
+      <c r="N21" s="55">
+        <v>0.78432167500000005</v>
+      </c>
+      <c r="O21" s="56">
+        <v>3.6462270000000001E-3</v>
+      </c>
+      <c r="P21" s="57">
+        <v>-4.3799191000000001E-2</v>
+      </c>
+      <c r="Q21" s="40">
+        <v>3.9525690000000004E-3</v>
+      </c>
+      <c r="R21">
+        <v>1</v>
+      </c>
+      <c r="S21" s="75"/>
+      <c r="T21" s="75"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A22" s="52" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22" s="44">
+        <v>3.697133279</v>
+      </c>
+      <c r="C22" s="47">
+        <v>-1.8153869999999999E-3</v>
+      </c>
+      <c r="D22" s="51">
+        <v>3.1511499999999998E-9</v>
+      </c>
+      <c r="E22" s="49">
+        <v>0.81829441999999997</v>
+      </c>
+      <c r="F22" s="50">
+        <v>0.80964177299999995</v>
+      </c>
+      <c r="G22" s="48">
+        <v>-0.73122531199999996</v>
+      </c>
+      <c r="H22" s="46">
+        <v>1.17668E-6</v>
+      </c>
+      <c r="I22" s="74" t="s">
+        <v>360</v>
+      </c>
+      <c r="K22" s="76" t="s">
+        <v>394</v>
+      </c>
+      <c r="L22" s="48">
+        <v>-2.4730867430000001</v>
+      </c>
+      <c r="M22" s="47">
+        <v>1.2572659999999999E-3</v>
+      </c>
+      <c r="N22" s="48">
+        <v>5.1304469999999998E-3</v>
+      </c>
+      <c r="O22" s="49">
+        <v>0.31728849799999997</v>
+      </c>
+      <c r="P22" s="50">
+        <v>0.284778427</v>
+      </c>
+      <c r="Q22" s="48">
+        <v>0.34387353100000001</v>
+      </c>
+      <c r="R22" s="45">
+        <v>2.3128867000000001E-2</v>
+      </c>
+      <c r="S22" s="75"/>
+      <c r="T22" s="75"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A23" s="73" t="s">
+        <v>361</v>
+      </c>
+      <c r="B23" s="40">
+        <v>0.10871773899999999</v>
+      </c>
+      <c r="C23" s="14">
+        <v>-3.5629500000000002E-5</v>
+      </c>
+      <c r="D23" s="40">
+        <v>0.94820806000000002</v>
+      </c>
+      <c r="E23" s="41">
+        <v>2.05744E-4</v>
+      </c>
+      <c r="F23" s="41">
+        <v>-4.7403505999999998E-2</v>
+      </c>
+      <c r="G23" s="40">
+        <v>-1.1857708E-2</v>
+      </c>
+      <c r="H23" s="40">
+        <v>0.95787459600000002</v>
+      </c>
+      <c r="I23" s="74" t="s">
+        <v>361</v>
+      </c>
+      <c r="K23" s="77" t="s">
+        <v>395</v>
+      </c>
+      <c r="L23" s="59">
+        <v>-2.4536090119999998</v>
+      </c>
+      <c r="M23" s="58">
+        <v>1.2248109999999999E-3</v>
+      </c>
+      <c r="N23" s="69">
+        <v>2.5473100000000001E-4</v>
+      </c>
+      <c r="O23" s="60">
+        <v>0.47872900000000002</v>
+      </c>
+      <c r="P23" s="60">
+        <v>0.45390657099999998</v>
+      </c>
+      <c r="Q23" s="59">
+        <v>0.51778662200000003</v>
+      </c>
+      <c r="R23" s="59">
+        <v>5.9616599999999997E-4</v>
+      </c>
+      <c r="S23" s="75"/>
+      <c r="T23" s="75"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A24" s="52" t="s">
+        <v>362</v>
+      </c>
+      <c r="B24" s="44">
+        <v>-0.68686740700000004</v>
+      </c>
+      <c r="C24" s="47">
+        <v>3.58594E-4</v>
+      </c>
+      <c r="D24" s="48">
+        <v>4.9703561E-2</v>
+      </c>
+      <c r="E24" s="49">
+        <v>0.17117596900000001</v>
+      </c>
+      <c r="F24" s="50">
+        <v>0.13170815799999999</v>
+      </c>
+      <c r="G24" s="40">
+        <v>0.24110673399999999</v>
+      </c>
+      <c r="H24" s="40">
+        <v>0.113050938</v>
+      </c>
+      <c r="I24" s="74" t="s">
+        <v>362</v>
+      </c>
+      <c r="K24" s="76" t="s">
+        <v>396</v>
+      </c>
+      <c r="L24" s="48">
+        <v>0.108082522</v>
+      </c>
+      <c r="M24" s="51">
+        <v>-3.4838200000000001E-5</v>
+      </c>
+      <c r="N24" s="48">
+        <v>0.838972567</v>
+      </c>
+      <c r="O24" s="49">
+        <v>2.011681E-3</v>
+      </c>
+      <c r="P24" s="50">
+        <v>-4.5511572E-2</v>
+      </c>
+      <c r="Q24" s="40">
+        <v>-1.9762848E-2</v>
+      </c>
+      <c r="R24" s="40">
+        <v>0.91586649399999998</v>
+      </c>
+      <c r="S24" s="75"/>
+      <c r="T24" s="75"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A25" s="73" t="s">
+        <v>363</v>
+      </c>
+      <c r="B25" s="40">
+        <v>1.1167735459999999</v>
+      </c>
+      <c r="C25" s="39">
+        <v>-5.1635799999999996E-4</v>
+      </c>
+      <c r="D25" s="40">
+        <v>0.32140079799999999</v>
+      </c>
+      <c r="E25" s="41">
+        <v>4.6812742999999997E-2</v>
+      </c>
+      <c r="F25" s="41">
+        <v>1.4228730000000001E-3</v>
+      </c>
+      <c r="G25" s="40">
+        <v>-0.15415020300000001</v>
+      </c>
+      <c r="H25" s="40">
+        <v>0.31557267900000002</v>
+      </c>
+      <c r="I25" s="74" t="s">
+        <v>363</v>
+      </c>
+      <c r="K25" s="77" t="s">
+        <v>397</v>
+      </c>
+      <c r="L25" s="40">
+        <v>-9.3546652999999994E-2</v>
+      </c>
+      <c r="M25" s="14">
+        <v>4.3538100000000002E-5</v>
+      </c>
+      <c r="N25" s="40">
+        <v>0.88769484399999998</v>
+      </c>
+      <c r="O25" s="41">
+        <v>9.7209300000000005E-4</v>
+      </c>
+      <c r="P25" s="41">
+        <v>-4.6600664999999999E-2</v>
+      </c>
+      <c r="Q25" s="40">
+        <v>3.5573124999999997E-2</v>
+      </c>
+      <c r="R25" s="40">
+        <v>0.83266591999999995</v>
+      </c>
+      <c r="S25" s="75"/>
+      <c r="T25" s="75"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="73" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="40">
+        <v>-0.82318983999999995</v>
+      </c>
+      <c r="C26" s="39">
+        <v>4.3709899999999998E-4</v>
+      </c>
+      <c r="D26" s="40">
+        <v>0.40334990300000001</v>
+      </c>
+      <c r="E26" s="41">
+        <v>3.3478521999999997E-2</v>
+      </c>
+      <c r="F26" s="41">
+        <v>-1.2546310999999999E-2</v>
+      </c>
+      <c r="G26" s="40">
+        <v>0.114624515</v>
+      </c>
+      <c r="H26" s="40">
+        <v>0.45960783999999999</v>
+      </c>
+      <c r="I26" s="74" t="s">
+        <v>70</v>
+      </c>
+      <c r="K26" s="76" t="s">
+        <v>398</v>
+      </c>
+      <c r="L26" s="59">
+        <v>-3.1727378480000001</v>
+      </c>
+      <c r="M26" s="58">
+        <v>1.604893E-3</v>
+      </c>
+      <c r="N26" s="69">
+        <v>2.9245600000000002E-4</v>
+      </c>
+      <c r="O26" s="60">
+        <v>0.472123599</v>
+      </c>
+      <c r="P26" s="60">
+        <v>0.44698662700000003</v>
+      </c>
+      <c r="Q26" s="59">
+        <v>0.53359687300000003</v>
+      </c>
+      <c r="R26" s="69">
+        <v>4.0161599999999998E-4</v>
+      </c>
+      <c r="S26" s="75"/>
+      <c r="T26" s="75"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="52" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="44">
+        <v>-2.4730867430000001</v>
+      </c>
+      <c r="C27" s="47">
+        <v>1.2572659999999999E-3</v>
+      </c>
+      <c r="D27" s="48">
+        <v>5.1304469999999998E-3</v>
+      </c>
+      <c r="E27" s="49">
+        <v>0.31728849799999997</v>
+      </c>
+      <c r="F27" s="50">
+        <v>0.284778427</v>
+      </c>
+      <c r="G27" s="44">
+        <v>0.34387353100000001</v>
+      </c>
+      <c r="H27" s="45">
+        <v>2.3128867000000001E-2</v>
+      </c>
+      <c r="I27" s="74" t="s">
+        <v>69</v>
+      </c>
+      <c r="K27" s="77" t="s">
+        <v>399</v>
+      </c>
+      <c r="L27" s="48">
+        <v>-2.842487363</v>
+      </c>
+      <c r="M27" s="47">
+        <v>1.41201E-3</v>
+      </c>
+      <c r="N27" s="51">
+        <v>1.05596E-5</v>
+      </c>
+      <c r="O27" s="49">
+        <v>0.61117614300000001</v>
+      </c>
+      <c r="P27" s="50">
+        <v>0.59266072199999997</v>
+      </c>
+      <c r="Q27" s="44">
+        <v>0.62055337399999999</v>
+      </c>
+      <c r="R27" s="46">
+        <v>3.7908599999999998E-5</v>
+      </c>
+      <c r="S27" s="75"/>
+      <c r="T27" s="75"/>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="73" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="40">
+        <v>0.108082522</v>
+      </c>
+      <c r="C28" s="14">
+        <v>-3.4838200000000001E-5</v>
+      </c>
+      <c r="D28" s="40">
+        <v>0.838972567</v>
+      </c>
+      <c r="E28" s="41">
+        <v>2.011681E-3</v>
+      </c>
+      <c r="F28" s="41">
+        <v>-4.5511572E-2</v>
+      </c>
+      <c r="G28" s="40">
+        <v>-1.9762848E-2</v>
+      </c>
+      <c r="H28" s="40">
+        <v>0.91586649399999998</v>
+      </c>
+      <c r="I28" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="K28" s="76" t="s">
+        <v>400</v>
+      </c>
+      <c r="L28" s="40">
+        <v>0.69638750999999999</v>
+      </c>
+      <c r="M28" s="39">
+        <v>-3.1844300000000001E-4</v>
+      </c>
+      <c r="N28" s="40">
+        <v>8.5344916000000007E-2</v>
+      </c>
+      <c r="O28" s="41">
+        <v>0.134378831</v>
+      </c>
+      <c r="P28" s="41">
+        <v>9.3158774999999999E-2</v>
+      </c>
+      <c r="Q28" s="40">
+        <v>-0.20158104600000001</v>
+      </c>
+      <c r="R28" s="40">
+        <v>0.18666048299999999</v>
+      </c>
+      <c r="S28" s="75"/>
+      <c r="T28" s="75"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" s="44">
+        <v>-3.1727378480000001</v>
+      </c>
+      <c r="C29" s="47">
+        <v>1.604893E-3</v>
+      </c>
+      <c r="D29" s="48">
+        <v>2.9245600000000002E-4</v>
+      </c>
+      <c r="E29" s="49">
+        <v>0.472123599</v>
+      </c>
+      <c r="F29" s="50">
+        <v>0.44698662700000003</v>
+      </c>
+      <c r="G29" s="44">
+        <v>0.53359687300000003</v>
+      </c>
+      <c r="H29" s="46">
+        <v>4.0161599999999998E-4</v>
+      </c>
+      <c r="I29" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="K29" s="77" t="s">
+        <v>401</v>
+      </c>
+      <c r="L29" s="48">
+        <v>-1.2682307159999999</v>
+      </c>
+      <c r="M29" s="47">
+        <v>6.3139100000000003E-4</v>
+      </c>
+      <c r="N29" s="48">
+        <v>2.4793835E-2</v>
+      </c>
+      <c r="O29" s="49">
+        <v>0.217743033</v>
+      </c>
+      <c r="P29" s="50">
+        <v>0.18049270100000001</v>
+      </c>
+      <c r="Q29" s="44">
+        <v>0.32015812399999999</v>
+      </c>
+      <c r="R29" s="45">
+        <v>3.4614801000000001E-2</v>
+      </c>
+      <c r="S29" s="75"/>
+      <c r="T29" s="75"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="73" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="40">
+        <v>0.69638750999999999</v>
+      </c>
+      <c r="C30" s="39">
+        <v>-3.1844300000000001E-4</v>
+      </c>
+      <c r="D30" s="40">
+        <v>8.5344916000000007E-2</v>
+      </c>
+      <c r="E30" s="41">
+        <v>0.134378831</v>
+      </c>
+      <c r="F30" s="41">
+        <v>9.3158774999999999E-2</v>
+      </c>
+      <c r="G30" s="40">
+        <v>-0.20158104600000001</v>
+      </c>
+      <c r="H30" s="40">
+        <v>0.18666048299999999</v>
+      </c>
+      <c r="I30" s="74" t="s">
+        <v>66</v>
+      </c>
+      <c r="K30" s="76" t="s">
+        <v>402</v>
+      </c>
+      <c r="L30" s="40">
+        <v>0.55243838999999995</v>
+      </c>
+      <c r="M30" s="39">
+        <v>-2.5535999999999999E-4</v>
+      </c>
+      <c r="N30" s="40">
+        <v>0.62783867299999996</v>
+      </c>
+      <c r="O30" s="41">
+        <v>1.139448E-2</v>
+      </c>
+      <c r="P30" s="41">
+        <v>-3.5681972999999999E-2</v>
+      </c>
+      <c r="Q30" s="40">
+        <v>-0.138339937</v>
+      </c>
+      <c r="R30" s="40">
+        <v>0.36920923</v>
+      </c>
+      <c r="S30" s="75"/>
+      <c r="T30" s="75"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="73" t="s">
+        <v>65</v>
+      </c>
+      <c r="B31" s="40">
+        <v>0.55243838999999995</v>
+      </c>
+      <c r="C31" s="39">
+        <v>-2.5535999999999999E-4</v>
+      </c>
+      <c r="D31" s="40">
+        <v>0.62783867299999996</v>
+      </c>
+      <c r="E31" s="41">
+        <v>1.139448E-2</v>
+      </c>
+      <c r="F31" s="41">
+        <v>-3.5681972999999999E-2</v>
+      </c>
+      <c r="G31" s="40">
+        <v>-0.138339937</v>
+      </c>
+      <c r="H31" s="40">
+        <v>0.36920923</v>
+      </c>
+      <c r="I31" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="K31" s="77" t="s">
+        <v>403</v>
+      </c>
+      <c r="L31" s="59">
+        <v>-1.868733872</v>
+      </c>
+      <c r="M31" s="58">
+        <v>9.5417799999999997E-4</v>
+      </c>
+      <c r="N31" s="59">
+        <v>8.0778229999999996E-3</v>
+      </c>
+      <c r="O31" s="60">
+        <v>0.28958943100000001</v>
+      </c>
+      <c r="P31" s="60">
+        <v>0.25576035600000002</v>
+      </c>
+      <c r="Q31" s="59">
+        <v>0.37549409299999997</v>
+      </c>
+      <c r="R31" s="59">
+        <v>1.3043404E-2</v>
+      </c>
+      <c r="S31" s="75"/>
+      <c r="T31" s="75"/>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>333</v>
+      </c>
+      <c r="C32" t="s">
+        <v>334</v>
+      </c>
+      <c r="D32" t="s">
+        <v>335</v>
+      </c>
+      <c r="E32" t="s">
+        <v>336</v>
+      </c>
+      <c r="F32" t="s">
+        <v>337</v>
+      </c>
+      <c r="G32" t="s">
+        <v>338</v>
+      </c>
+      <c r="H32" t="s">
+        <v>339</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="T4:T33">
+    <sortCondition ref="T4:T33"/>
+  </sortState>
+  <conditionalFormatting sqref="D2:D31">
+    <cfRule type="cellIs" dxfId="3" priority="10" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E31">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F31">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H31">
+    <cfRule type="cellIs" dxfId="2" priority="7" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G31">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N2:N31">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:O31">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P2:P31">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="R2:R31">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q2:Q31">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="-1"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF5A8AC6"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
he solucionado el error del Mann-Kendall y he añadido los nombres correctamente
</commit_message>
<xml_diff>
--- a/R/ResultadosR_LSWI.xlsx
+++ b/R/ResultadosR_LSWI.xlsx
@@ -20,7 +20,7 @@
     <sheet name="Resultados 27-08" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Resultados 27-08'!$L$1:$O$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Resultados 27-08'!$L$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="436">
   <si>
     <t>Dado que el p-valor es menor que 0.05, rechazamos la hipótesis nula de que no hay tendencia monotónica en la serie de tiempo. Esto significa que hay evidencia estadísticamente significativa para concluir que existe una tendencia monotónica en la serie de tiempo.</t>
   </si>
@@ -1569,7 +1569,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1931,13 +1931,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2060,28 +2075,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2090,43 +2087,49 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
     <cellStyle name="Salida" xfId="2" builtinId="21"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -55965,7 +55968,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B34:G37">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -55994,7 +55997,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B21:P24">
-    <cfRule type="cellIs" dxfId="8" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -56032,7 +56035,7 @@
   <dimension ref="A1:AA32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="L2" sqref="L2:N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -56043,10 +56046,12 @@
     <col min="6" max="6" width="13" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.28515625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="43" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="18" thickBot="1">
@@ -56071,17 +56076,20 @@
       <c r="H1" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="94" t="s">
         <v>371</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="94" t="s">
         <v>368</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="95" t="s">
         <v>369</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="34" t="s">
         <v>435</v>
+      </c>
+      <c r="P1" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="S1" t="s">
         <v>434</v>
@@ -56139,17 +56147,20 @@
       <c r="I2" s="71" t="s">
         <v>340</v>
       </c>
-      <c r="L2" s="76" t="s">
-        <v>404</v>
-      </c>
-      <c r="M2" s="87">
-        <v>0.38339921799999999</v>
-      </c>
-      <c r="N2" s="84">
-        <v>1.123178E-2</v>
-      </c>
-      <c r="O2" s="77" t="s">
-        <v>355</v>
+      <c r="L2" s="90" t="s">
+        <v>375</v>
+      </c>
+      <c r="M2" s="81">
+        <v>0.185770765</v>
+      </c>
+      <c r="N2" s="78">
+        <v>0.22441148799999999</v>
+      </c>
+      <c r="O2" s="84" t="s">
+        <v>340</v>
+      </c>
+      <c r="P2" s="86" t="s">
+        <v>419</v>
       </c>
       <c r="T2" s="74" t="s">
         <v>374</v>
@@ -56204,17 +56215,20 @@
       <c r="I3" s="71" t="s">
         <v>341</v>
       </c>
-      <c r="L3" s="78" t="s">
-        <v>419</v>
-      </c>
-      <c r="M3" s="88">
-        <v>0.185770765</v>
-      </c>
-      <c r="N3" s="85">
-        <v>0.22441148799999999</v>
-      </c>
-      <c r="O3" s="79" t="s">
-        <v>340</v>
+      <c r="L3" s="91" t="s">
+        <v>374</v>
+      </c>
+      <c r="M3" s="82">
+        <v>0.38339921799999999</v>
+      </c>
+      <c r="N3" s="79">
+        <v>1.123178E-2</v>
+      </c>
+      <c r="O3" s="77" t="s">
+        <v>355</v>
+      </c>
+      <c r="P3" s="87" t="s">
+        <v>404</v>
       </c>
       <c r="T3" s="75" t="s">
         <v>375</v>
@@ -56269,17 +56283,20 @@
       <c r="I4" s="71" t="s">
         <v>342</v>
       </c>
-      <c r="L4" s="80" t="s">
-        <v>405</v>
-      </c>
-      <c r="M4" s="88">
-        <v>5.9288542999999999E-2</v>
-      </c>
-      <c r="N4" s="85">
-        <v>0.71157145499999996</v>
-      </c>
-      <c r="O4" s="81" t="s">
-        <v>356</v>
+      <c r="L4" s="92" t="s">
+        <v>377</v>
+      </c>
+      <c r="M4" s="82">
+        <v>9.0909093999999996E-2</v>
+      </c>
+      <c r="N4" s="79">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="O4" s="76" t="s">
+        <v>341</v>
+      </c>
+      <c r="P4" s="88" t="s">
+        <v>421</v>
       </c>
       <c r="T4" s="74" t="s">
         <v>376</v>
@@ -56334,17 +56351,20 @@
       <c r="I5" s="71" t="s">
         <v>343</v>
       </c>
-      <c r="L5" s="78" t="s">
-        <v>421</v>
-      </c>
-      <c r="M5" s="88">
-        <v>9.0909093999999996E-2</v>
-      </c>
-      <c r="N5" s="85">
-        <v>0.56122016900000005</v>
-      </c>
-      <c r="O5" s="79" t="s">
-        <v>341</v>
+      <c r="L5" s="91" t="s">
+        <v>376</v>
+      </c>
+      <c r="M5" s="82">
+        <v>5.9288542999999999E-2</v>
+      </c>
+      <c r="N5" s="79">
+        <v>0.71157145499999996</v>
+      </c>
+      <c r="O5" s="77" t="s">
+        <v>356</v>
+      </c>
+      <c r="P5" s="87" t="s">
+        <v>405</v>
       </c>
       <c r="T5" s="75" t="s">
         <v>377</v>
@@ -56399,17 +56419,20 @@
       <c r="I6" s="71" t="s">
         <v>344</v>
       </c>
-      <c r="L6" s="80" t="s">
-        <v>406</v>
-      </c>
-      <c r="M6" s="88">
-        <v>-9.0909093999999996E-2</v>
-      </c>
-      <c r="N6" s="85">
-        <v>0.56122016900000005</v>
-      </c>
-      <c r="O6" s="81" t="s">
-        <v>357</v>
+      <c r="L6" s="92" t="s">
+        <v>379</v>
+      </c>
+      <c r="M6" s="82">
+        <v>-3.9525690000000004E-3</v>
+      </c>
+      <c r="N6" s="25">
+        <v>1</v>
+      </c>
+      <c r="O6" s="76" t="s">
+        <v>342</v>
+      </c>
+      <c r="P6" s="88" t="s">
+        <v>423</v>
       </c>
       <c r="T6" s="74" t="s">
         <v>378</v>
@@ -56464,17 +56487,20 @@
       <c r="I7" s="71" t="s">
         <v>345</v>
       </c>
-      <c r="L7" s="78" t="s">
-        <v>423</v>
-      </c>
-      <c r="M7" s="88">
-        <v>-3.9525690000000004E-3</v>
-      </c>
-      <c r="N7" s="25">
-        <v>1</v>
-      </c>
-      <c r="O7" s="79" t="s">
-        <v>342</v>
+      <c r="L7" s="91" t="s">
+        <v>378</v>
+      </c>
+      <c r="M7" s="82">
+        <v>-9.0909093999999996E-2</v>
+      </c>
+      <c r="N7" s="79">
+        <v>0.56122016900000005</v>
+      </c>
+      <c r="O7" s="77" t="s">
+        <v>357</v>
+      </c>
+      <c r="P7" s="87" t="s">
+        <v>406</v>
       </c>
       <c r="T7" s="75" t="s">
         <v>379</v>
@@ -56529,17 +56555,20 @@
       <c r="I8" s="71" t="s">
         <v>346</v>
       </c>
-      <c r="L8" s="80" t="s">
-        <v>407</v>
-      </c>
-      <c r="M8" s="88">
-        <v>-0.10671937500000001</v>
-      </c>
-      <c r="N8" s="85">
-        <v>0.492289484</v>
-      </c>
-      <c r="O8" s="81" t="s">
-        <v>358</v>
+      <c r="L8" s="92" t="s">
+        <v>381</v>
+      </c>
+      <c r="M8" s="82">
+        <v>0.28853756200000003</v>
+      </c>
+      <c r="N8" s="79">
+        <v>5.7229637999999999E-2</v>
+      </c>
+      <c r="O8" s="76" t="s">
+        <v>343</v>
+      </c>
+      <c r="P8" s="88" t="s">
+        <v>425</v>
       </c>
       <c r="T8" s="74" t="s">
         <v>380</v>
@@ -56594,17 +56623,20 @@
       <c r="I9" s="71" t="s">
         <v>347</v>
       </c>
-      <c r="L9" s="78" t="s">
-        <v>425</v>
-      </c>
-      <c r="M9" s="88">
-        <v>0.28853756200000003</v>
-      </c>
-      <c r="N9" s="85">
-        <v>5.7229637999999999E-2</v>
-      </c>
-      <c r="O9" s="79" t="s">
-        <v>343</v>
+      <c r="L9" s="91" t="s">
+        <v>380</v>
+      </c>
+      <c r="M9" s="82">
+        <v>-0.10671937500000001</v>
+      </c>
+      <c r="N9" s="79">
+        <v>0.492289484</v>
+      </c>
+      <c r="O9" s="77" t="s">
+        <v>358</v>
+      </c>
+      <c r="P9" s="87" t="s">
+        <v>407</v>
       </c>
       <c r="T9" s="75" t="s">
         <v>381</v>
@@ -56659,17 +56691,20 @@
       <c r="I10" s="71" t="s">
         <v>348</v>
       </c>
-      <c r="L10" s="80" t="s">
-        <v>408</v>
-      </c>
-      <c r="M10" s="88">
-        <v>0.23320159300000001</v>
-      </c>
-      <c r="N10" s="85">
-        <v>0.125570178</v>
-      </c>
-      <c r="O10" s="81" t="s">
-        <v>359</v>
+      <c r="L10" s="92" t="s">
+        <v>383</v>
+      </c>
+      <c r="M10" s="82">
+        <v>6.7193680000000006E-2</v>
+      </c>
+      <c r="N10" s="79">
+        <v>0.67261099800000002</v>
+      </c>
+      <c r="O10" s="76" t="s">
+        <v>345</v>
+      </c>
+      <c r="P10" s="88" t="s">
+        <v>429</v>
       </c>
       <c r="T10" s="74" t="s">
         <v>382</v>
@@ -56724,17 +56759,20 @@
       <c r="I11" s="71" t="s">
         <v>349</v>
       </c>
-      <c r="L11" s="78" t="s">
-        <v>427</v>
-      </c>
-      <c r="M11" s="88">
-        <v>0.264822155</v>
-      </c>
-      <c r="N11" s="85">
-        <v>8.1317901999999997E-2</v>
-      </c>
-      <c r="O11" s="79" t="s">
-        <v>344</v>
+      <c r="L11" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="M11" s="82">
+        <v>-0.73122531199999996</v>
+      </c>
+      <c r="N11" s="36">
+        <v>1.17668E-6</v>
+      </c>
+      <c r="O11" s="77" t="s">
+        <v>360</v>
+      </c>
+      <c r="P11" s="87" t="s">
+        <v>409</v>
       </c>
       <c r="T11" s="75" t="s">
         <v>383</v>
@@ -56789,17 +56827,20 @@
       <c r="I12" s="71" t="s">
         <v>350</v>
       </c>
-      <c r="L12" s="80" t="s">
-        <v>409</v>
-      </c>
-      <c r="M12" s="88">
-        <v>-0.73122531199999996</v>
-      </c>
-      <c r="N12" s="36">
-        <v>1.17668E-6</v>
-      </c>
-      <c r="O12" s="81" t="s">
-        <v>360</v>
+      <c r="L12" s="92" t="s">
+        <v>385</v>
+      </c>
+      <c r="M12" s="82">
+        <v>0.264822155</v>
+      </c>
+      <c r="N12" s="79">
+        <v>8.1317901999999997E-2</v>
+      </c>
+      <c r="O12" s="76" t="s">
+        <v>344</v>
+      </c>
+      <c r="P12" s="88" t="s">
+        <v>427</v>
       </c>
       <c r="T12" s="74" t="s">
         <v>384</v>
@@ -56854,17 +56895,20 @@
       <c r="I13" s="71" t="s">
         <v>351</v>
       </c>
-      <c r="L13" s="78" t="s">
-        <v>429</v>
-      </c>
-      <c r="M13" s="88">
-        <v>6.7193680000000006E-2</v>
-      </c>
-      <c r="N13" s="85">
-        <v>0.67261099800000002</v>
-      </c>
-      <c r="O13" s="79" t="s">
-        <v>345</v>
+      <c r="L13" s="91" t="s">
+        <v>384</v>
+      </c>
+      <c r="M13" s="82">
+        <v>0.23320159300000001</v>
+      </c>
+      <c r="N13" s="79">
+        <v>0.125570178</v>
+      </c>
+      <c r="O13" s="77" t="s">
+        <v>359</v>
+      </c>
+      <c r="P13" s="87" t="s">
+        <v>408</v>
       </c>
       <c r="T13" s="75" t="s">
         <v>385</v>
@@ -56919,17 +56963,20 @@
       <c r="I14" s="71" t="s">
         <v>352</v>
       </c>
-      <c r="L14" s="80" t="s">
-        <v>410</v>
-      </c>
-      <c r="M14" s="88">
-        <v>-1.1857708E-2</v>
-      </c>
-      <c r="N14" s="85">
-        <v>0.95787459600000002</v>
-      </c>
-      <c r="O14" s="81" t="s">
-        <v>361</v>
+      <c r="L14" s="92" t="s">
+        <v>387</v>
+      </c>
+      <c r="M14" s="82">
+        <v>0.122529648</v>
+      </c>
+      <c r="N14" s="79">
+        <v>0.42817783399999998</v>
+      </c>
+      <c r="O14" s="76" t="s">
+        <v>346</v>
+      </c>
+      <c r="P14" s="88" t="s">
+        <v>430</v>
       </c>
       <c r="T14" s="74" t="s">
         <v>386</v>
@@ -56984,17 +57031,20 @@
       <c r="I15" s="71" t="s">
         <v>353</v>
       </c>
-      <c r="L15" s="78" t="s">
-        <v>430</v>
-      </c>
-      <c r="M15" s="88">
-        <v>0.122529648</v>
-      </c>
-      <c r="N15" s="85">
-        <v>0.42817783399999998</v>
-      </c>
-      <c r="O15" s="79" t="s">
-        <v>346</v>
+      <c r="L15" s="91" t="s">
+        <v>386</v>
+      </c>
+      <c r="M15" s="82">
+        <v>-1.1857708E-2</v>
+      </c>
+      <c r="N15" s="79">
+        <v>0.95787459600000002</v>
+      </c>
+      <c r="O15" s="77" t="s">
+        <v>361</v>
+      </c>
+      <c r="P15" s="87" t="s">
+        <v>410</v>
       </c>
       <c r="T15" s="75" t="s">
         <v>387</v>
@@ -57049,17 +57099,20 @@
       <c r="I16" s="71" t="s">
         <v>354</v>
       </c>
-      <c r="L16" s="80" t="s">
-        <v>411</v>
-      </c>
-      <c r="M16" s="88">
-        <v>0.24110673399999999</v>
-      </c>
-      <c r="N16" s="85">
-        <v>0.113050938</v>
-      </c>
-      <c r="O16" s="81" t="s">
-        <v>362</v>
+      <c r="L16" s="92" t="s">
+        <v>389</v>
+      </c>
+      <c r="M16" s="82">
+        <v>0.58893281200000003</v>
+      </c>
+      <c r="N16" s="36">
+        <v>9.2744799999999993E-5</v>
+      </c>
+      <c r="O16" s="76" t="s">
+        <v>347</v>
+      </c>
+      <c r="P16" s="88" t="s">
+        <v>431</v>
       </c>
       <c r="T16" s="74" t="s">
         <v>388</v>
@@ -57114,17 +57167,20 @@
       <c r="I17" s="73" t="s">
         <v>355</v>
       </c>
-      <c r="L17" s="78" t="s">
-        <v>431</v>
-      </c>
-      <c r="M17" s="88">
-        <v>0.58893281200000003</v>
-      </c>
-      <c r="N17" s="36">
-        <v>9.2744799999999993E-5</v>
-      </c>
-      <c r="O17" s="79" t="s">
-        <v>347</v>
+      <c r="L17" s="91" t="s">
+        <v>388</v>
+      </c>
+      <c r="M17" s="82">
+        <v>0.24110673399999999</v>
+      </c>
+      <c r="N17" s="79">
+        <v>0.113050938</v>
+      </c>
+      <c r="O17" s="77" t="s">
+        <v>362</v>
+      </c>
+      <c r="P17" s="87" t="s">
+        <v>411</v>
       </c>
       <c r="T17" s="75" t="s">
         <v>389</v>
@@ -57179,17 +57235,20 @@
       <c r="I18" s="73" t="s">
         <v>356</v>
       </c>
-      <c r="L18" s="80" t="s">
-        <v>412</v>
-      </c>
-      <c r="M18" s="88">
-        <v>-0.15415020300000001</v>
-      </c>
-      <c r="N18" s="85">
-        <v>0.31557267900000002</v>
-      </c>
-      <c r="O18" s="81" t="s">
-        <v>363</v>
+      <c r="L18" s="92" t="s">
+        <v>391</v>
+      </c>
+      <c r="M18" s="82">
+        <v>0.35177868600000001</v>
+      </c>
+      <c r="N18" s="79">
+        <v>2.0119070999999999E-2</v>
+      </c>
+      <c r="O18" s="76" t="s">
+        <v>348</v>
+      </c>
+      <c r="P18" s="88" t="s">
+        <v>432</v>
       </c>
       <c r="T18" s="74" t="s">
         <v>390</v>
@@ -57244,17 +57303,20 @@
       <c r="I19" s="73" t="s">
         <v>357</v>
       </c>
-      <c r="L19" s="78" t="s">
-        <v>432</v>
-      </c>
-      <c r="M19" s="88">
-        <v>0.35177868600000001</v>
-      </c>
-      <c r="N19" s="85">
-        <v>2.0119070999999999E-2</v>
-      </c>
-      <c r="O19" s="79" t="s">
-        <v>348</v>
+      <c r="L19" s="91" t="s">
+        <v>390</v>
+      </c>
+      <c r="M19" s="82">
+        <v>-0.15415020300000001</v>
+      </c>
+      <c r="N19" s="79">
+        <v>0.31557267900000002</v>
+      </c>
+      <c r="O19" s="77" t="s">
+        <v>363</v>
+      </c>
+      <c r="P19" s="87" t="s">
+        <v>412</v>
       </c>
       <c r="T19" s="75" t="s">
         <v>391</v>
@@ -57309,17 +57371,20 @@
       <c r="I20" s="73" t="s">
         <v>358</v>
       </c>
-      <c r="L20" s="80" t="s">
-        <v>413</v>
-      </c>
-      <c r="M20" s="88">
-        <v>0.114624515</v>
-      </c>
-      <c r="N20" s="85">
-        <v>0.45960783999999999</v>
-      </c>
-      <c r="O20" s="81" t="s">
-        <v>70</v>
+      <c r="L20" s="92" t="s">
+        <v>393</v>
+      </c>
+      <c r="M20" s="82">
+        <v>3.9525690000000004E-3</v>
+      </c>
+      <c r="N20" s="25">
+        <v>1</v>
+      </c>
+      <c r="O20" s="76" t="s">
+        <v>349</v>
+      </c>
+      <c r="P20" s="88" t="s">
+        <v>433</v>
       </c>
       <c r="T20" s="74" t="s">
         <v>392</v>
@@ -57374,17 +57439,20 @@
       <c r="I21" s="73" t="s">
         <v>359</v>
       </c>
-      <c r="L21" s="78" t="s">
-        <v>433</v>
-      </c>
-      <c r="M21" s="88">
-        <v>3.9525690000000004E-3</v>
-      </c>
-      <c r="N21" s="25">
-        <v>1</v>
-      </c>
-      <c r="O21" s="79" t="s">
-        <v>349</v>
+      <c r="L21" s="91" t="s">
+        <v>392</v>
+      </c>
+      <c r="M21" s="82">
+        <v>0.114624515</v>
+      </c>
+      <c r="N21" s="79">
+        <v>0.45960783999999999</v>
+      </c>
+      <c r="O21" s="77" t="s">
+        <v>70</v>
+      </c>
+      <c r="P21" s="87" t="s">
+        <v>413</v>
       </c>
       <c r="T21" s="75" t="s">
         <v>393</v>
@@ -57439,17 +57507,20 @@
       <c r="I22" s="73" t="s">
         <v>360</v>
       </c>
-      <c r="L22" s="80" t="s">
-        <v>414</v>
-      </c>
-      <c r="M22" s="88">
-        <v>0.34387353100000001</v>
-      </c>
-      <c r="N22" s="85">
-        <v>2.3128867000000001E-2</v>
-      </c>
-      <c r="O22" s="81" t="s">
-        <v>69</v>
+      <c r="L22" s="92" t="s">
+        <v>395</v>
+      </c>
+      <c r="M22" s="82">
+        <v>0.51778662200000003</v>
+      </c>
+      <c r="N22" s="79">
+        <v>5.9616599999999997E-4</v>
+      </c>
+      <c r="O22" s="76" t="s">
+        <v>350</v>
+      </c>
+      <c r="P22" s="88" t="s">
+        <v>420</v>
       </c>
       <c r="T22" s="74" t="s">
         <v>394</v>
@@ -57504,17 +57575,20 @@
       <c r="I23" s="73" t="s">
         <v>361</v>
       </c>
-      <c r="L23" s="78" t="s">
-        <v>420</v>
-      </c>
-      <c r="M23" s="88">
-        <v>0.51778662200000003</v>
-      </c>
-      <c r="N23" s="85">
-        <v>5.9616599999999997E-4</v>
-      </c>
-      <c r="O23" s="79" t="s">
-        <v>350</v>
+      <c r="L23" s="91" t="s">
+        <v>394</v>
+      </c>
+      <c r="M23" s="82">
+        <v>0.34387353100000001</v>
+      </c>
+      <c r="N23" s="79">
+        <v>2.3128867000000001E-2</v>
+      </c>
+      <c r="O23" s="77" t="s">
+        <v>69</v>
+      </c>
+      <c r="P23" s="87" t="s">
+        <v>414</v>
       </c>
       <c r="T23" s="75" t="s">
         <v>395</v>
@@ -57569,17 +57643,20 @@
       <c r="I24" s="73" t="s">
         <v>362</v>
       </c>
-      <c r="L24" s="80" t="s">
-        <v>415</v>
-      </c>
-      <c r="M24" s="88">
-        <v>-1.9762848E-2</v>
-      </c>
-      <c r="N24" s="85">
-        <v>0.91586649399999998</v>
-      </c>
-      <c r="O24" s="81" t="s">
-        <v>68</v>
+      <c r="L24" s="92" t="s">
+        <v>397</v>
+      </c>
+      <c r="M24" s="82">
+        <v>0.37549409299999997</v>
+      </c>
+      <c r="N24" s="79">
+        <v>1.3043404E-2</v>
+      </c>
+      <c r="O24" s="76" t="s">
+        <v>354</v>
+      </c>
+      <c r="P24" s="88" t="s">
+        <v>428</v>
       </c>
       <c r="T24" s="74" t="s">
         <v>396</v>
@@ -57634,17 +57711,20 @@
       <c r="I25" s="73" t="s">
         <v>363</v>
       </c>
-      <c r="L25" s="78" t="s">
-        <v>422</v>
-      </c>
-      <c r="M25" s="88">
-        <v>3.5573124999999997E-2</v>
-      </c>
-      <c r="N25" s="85">
-        <v>0.83266591999999995</v>
-      </c>
-      <c r="O25" s="79" t="s">
-        <v>351</v>
+      <c r="L25" s="91" t="s">
+        <v>396</v>
+      </c>
+      <c r="M25" s="82">
+        <v>-0.138339937</v>
+      </c>
+      <c r="N25" s="79">
+        <v>0.36920923</v>
+      </c>
+      <c r="O25" s="77" t="s">
+        <v>65</v>
+      </c>
+      <c r="P25" s="87" t="s">
+        <v>418</v>
       </c>
       <c r="T25" s="75" t="s">
         <v>397</v>
@@ -57699,17 +57779,20 @@
       <c r="I26" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="L26" s="80" t="s">
-        <v>416</v>
-      </c>
-      <c r="M26" s="88">
-        <v>0.53359687300000003</v>
+      <c r="L26" s="92" t="s">
+        <v>399</v>
+      </c>
+      <c r="M26" s="82">
+        <v>0.62055337399999999</v>
       </c>
       <c r="N26" s="36">
-        <v>4.0161599999999998E-4</v>
-      </c>
-      <c r="O26" s="81" t="s">
-        <v>67</v>
+        <v>3.7908599999999998E-5</v>
+      </c>
+      <c r="O26" s="76" t="s">
+        <v>352</v>
+      </c>
+      <c r="P26" s="88" t="s">
+        <v>424</v>
       </c>
       <c r="T26" s="74" t="s">
         <v>398</v>
@@ -57764,17 +57847,20 @@
       <c r="I27" s="73" t="s">
         <v>69</v>
       </c>
-      <c r="L27" s="78" t="s">
-        <v>424</v>
-      </c>
-      <c r="M27" s="88">
-        <v>0.62055337399999999</v>
+      <c r="L27" s="91" t="s">
+        <v>398</v>
+      </c>
+      <c r="M27" s="82">
+        <v>0.53359687300000003</v>
       </c>
       <c r="N27" s="36">
-        <v>3.7908599999999998E-5</v>
-      </c>
-      <c r="O27" s="79" t="s">
-        <v>352</v>
+        <v>4.0161599999999998E-4</v>
+      </c>
+      <c r="O27" s="77" t="s">
+        <v>67</v>
+      </c>
+      <c r="P27" s="87" t="s">
+        <v>416</v>
       </c>
       <c r="T27" s="75" t="s">
         <v>399</v>
@@ -57829,17 +57915,20 @@
       <c r="I28" s="73" t="s">
         <v>68</v>
       </c>
-      <c r="L28" s="80" t="s">
-        <v>417</v>
-      </c>
-      <c r="M28" s="88">
-        <v>-0.20158104600000001</v>
-      </c>
-      <c r="N28" s="85">
-        <v>0.18666048299999999</v>
-      </c>
-      <c r="O28" s="81" t="s">
-        <v>66</v>
+      <c r="L28" s="92" t="s">
+        <v>401</v>
+      </c>
+      <c r="M28" s="82">
+        <v>3.5573124999999997E-2</v>
+      </c>
+      <c r="N28" s="79">
+        <v>0.83266591999999995</v>
+      </c>
+      <c r="O28" s="76" t="s">
+        <v>351</v>
+      </c>
+      <c r="P28" s="88" t="s">
+        <v>422</v>
       </c>
       <c r="T28" s="74" t="s">
         <v>400</v>
@@ -57894,17 +57983,20 @@
       <c r="I29" s="73" t="s">
         <v>67</v>
       </c>
-      <c r="L29" s="78" t="s">
-        <v>426</v>
-      </c>
-      <c r="M29" s="88">
-        <v>0.32015812399999999</v>
-      </c>
-      <c r="N29" s="85">
-        <v>3.4614801000000001E-2</v>
-      </c>
-      <c r="O29" s="79" t="s">
-        <v>353</v>
+      <c r="L29" s="91" t="s">
+        <v>400</v>
+      </c>
+      <c r="M29" s="82">
+        <v>-1.9762848E-2</v>
+      </c>
+      <c r="N29" s="79">
+        <v>0.91586649399999998</v>
+      </c>
+      <c r="O29" s="77" t="s">
+        <v>68</v>
+      </c>
+      <c r="P29" s="87" t="s">
+        <v>415</v>
       </c>
       <c r="T29" s="75" t="s">
         <v>401</v>
@@ -57959,17 +58051,20 @@
       <c r="I30" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="L30" s="80" t="s">
-        <v>418</v>
-      </c>
-      <c r="M30" s="88">
-        <v>-0.138339937</v>
-      </c>
-      <c r="N30" s="85">
-        <v>0.36920923</v>
-      </c>
-      <c r="O30" s="81" t="s">
-        <v>65</v>
+      <c r="L30" s="92" t="s">
+        <v>403</v>
+      </c>
+      <c r="M30" s="82">
+        <v>0.32015812399999999</v>
+      </c>
+      <c r="N30" s="79">
+        <v>3.4614801000000001E-2</v>
+      </c>
+      <c r="O30" s="76" t="s">
+        <v>353</v>
+      </c>
+      <c r="P30" s="88" t="s">
+        <v>426</v>
       </c>
       <c r="T30" s="74" t="s">
         <v>402</v>
@@ -58024,17 +58119,20 @@
       <c r="I31" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="L31" s="82" t="s">
-        <v>428</v>
-      </c>
-      <c r="M31" s="89">
-        <v>0.37549409299999997</v>
-      </c>
-      <c r="N31" s="86">
-        <v>1.3043404E-2</v>
-      </c>
-      <c r="O31" s="83" t="s">
-        <v>354</v>
+      <c r="L31" s="93" t="s">
+        <v>402</v>
+      </c>
+      <c r="M31" s="83">
+        <v>-0.20158104600000001</v>
+      </c>
+      <c r="N31" s="80">
+        <v>0.18666048299999999</v>
+      </c>
+      <c r="O31" s="85" t="s">
+        <v>66</v>
+      </c>
+      <c r="P31" s="89" t="s">
+        <v>417</v>
       </c>
       <c r="T31" s="75" t="s">
         <v>403</v>
@@ -58085,16 +58183,16 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="L1:O1">
-    <sortState ref="L2:O31">
-      <sortCondition ref="O1"/>
+  <autoFilter ref="L1:P1">
+    <sortState ref="L2:P31">
+      <sortCondition ref="L1"/>
     </sortState>
   </autoFilter>
   <sortState ref="O4:O33">
     <sortCondition ref="O4:O33"/>
   </sortState>
   <conditionalFormatting sqref="D2:D31">
-    <cfRule type="cellIs" dxfId="7" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58119,7 +58217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="6" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58136,7 +58234,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="5" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="15" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58161,7 +58259,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA2:AA31">
-    <cfRule type="cellIs" dxfId="4" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="12" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58178,7 +58276,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>